<commit_message>
doc: add desc for fuel ecosystems
</commit_message>
<xml_diff>
--- a/并行EVM主要叙事项目市场规模统计.xlsx
+++ b/并行EVM主要叙事项目市场规模统计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24800" windowHeight="11140" activeTab="1"/>
+    <workbookView windowWidth="27800" windowHeight="13140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1739,7 +1739,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
doc: tech implement path
</commit_message>
<xml_diff>
--- a/并行EVM主要叙事项目市场规模统计.xlsx
+++ b/并行EVM主要叙事项目市场规模统计.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27800" windowHeight="13140" activeTab="1"/>
+    <workbookView windowWidth="27660" windowHeight="13160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t>名称</t>
   </si>
@@ -213,6 +215,99 @@
   </si>
   <si>
     <t>Monad Homepage</t>
+  </si>
+  <si>
+    <t>步骤</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>&lt; 2</t>
+  </si>
+  <si>
+    <t>&lt; 0</t>
+  </si>
+  <si>
+    <t>从账本中读取A的账户余额和C的账户余额</t>
+  </si>
+  <si>
+    <t>2-0.5</t>
+  </si>
+  <si>
+    <t>0+0.5</t>
+  </si>
+  <si>
+    <t>计算收支平衡：A账户余额减去0.5，C账户余额增加0.5</t>
+  </si>
+  <si>
+    <t>&gt; 1.5</t>
+  </si>
+  <si>
+    <t>&gt; 0.5</t>
+  </si>
+  <si>
+    <t>将A和C的账户余额更新回账本</t>
+  </si>
+  <si>
+    <t>&lt; 1</t>
+  </si>
+  <si>
+    <t>&lt; 0.5</t>
+  </si>
+  <si>
+    <t>从账本中读取B的账户余额和C的账户余额</t>
+  </si>
+  <si>
+    <t>1-0.5</t>
+  </si>
+  <si>
+    <t>0.5+0.5</t>
+  </si>
+  <si>
+    <t>计算收支平衡：B账户余额减去0.5，C账户余额增加 0.5</t>
+  </si>
+  <si>
+    <t>&gt; 1</t>
+  </si>
+  <si>
+    <t>将B和C的账户余额更新回账本</t>
+  </si>
+  <si>
+    <t>并行任务1：从账本中读取A和C的账户余额</t>
+  </si>
+  <si>
+    <t>并行任务1：计算收支平衡，A账户余额减去0.5，C账户余额增加0.5</t>
+  </si>
+  <si>
+    <t>*3</t>
+  </si>
+  <si>
+    <t>并行任务2：从账本中读取B和C的账户余额（注意，还是0！）</t>
+  </si>
+  <si>
+    <t>并行任务1：将A和C的账户余额更新回账本</t>
+  </si>
+  <si>
+    <t>*5</t>
+  </si>
+  <si>
+    <t>并行任务2：计算收支平衡，B账户余额减去0.5，C账户余额增加0.5</t>
+  </si>
+  <si>
+    <t>*6</t>
+  </si>
+  <si>
+    <t>并行任务2：将B和C的账户余额更新回账本</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1833,7 @@
   <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
@@ -1967,4 +2062,282 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="4"/>
+  <cols>
+    <col min="5" max="5" width="52.7115384615385" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="4"/>
+  <cols>
+    <col min="5" max="5" width="71.0769230769231" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>